<commit_message>
New Code with changes
</commit_message>
<xml_diff>
--- a/JulyMaven01/src/test/java/excelsheet/testdata.xlsx
+++ b/JulyMaven01/src/test/java/excelsheet/testdata.xlsx
@@ -14,26 +14,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>pass1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Current Price (Rs)</t>
+  </si>
+  <si>
+    <t>Brigade Enterprises Ltd.</t>
+  </si>
+  <si>
+    <t>DLF Ltd.</t>
+  </si>
+  <si>
+    <t>Godrej Properties Ltd.</t>
+  </si>
+  <si>
+    <t>Indiabulls Real Estate Ltd.</t>
+  </si>
+  <si>
+    <t>Mahindra Lifespace Developers Ltd.</t>
+  </si>
+  <si>
+    <t>Oberoi Realty Ltd.</t>
+  </si>
+  <si>
+    <t>Phoenix Mills Ltd.</t>
+  </si>
+  <si>
+    <t>Prestige Estates Projects Ltd.</t>
+  </si>
+  <si>
+    <t>Sobha Ltd.</t>
+  </si>
+  <si>
+    <t>Sunteck Realty Ltd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,28 +400,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>139.80000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3">
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>55.55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>212.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>352.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>595.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>215.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>190.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>